<commit_message>
Assigned the tasks for the test plan revision
</commit_message>
<xml_diff>
--- a/TestPlan/Notes.xlsx
+++ b/TestPlan/Notes.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dimitar Panayotov\Dropbox\Git\Team Lich\TestsAndPlans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TestsAndPlans\TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,10 @@
   <sheets>
     <sheet name="Notes (04.12.2015)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,25 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t xml:space="preserve"> Да се добави Probabiliy</t>
-  </si>
-  <si>
-    <t>Parse/Fail Criteria - Излишни</t>
-  </si>
-  <si>
-    <t>Да се добави Owner на риска</t>
-  </si>
-  <si>
-    <t>Да се опишат Severity-тата</t>
-  </si>
-  <si>
-    <t>Regression Testing - Трябва да се изпълнява регулярно</t>
-  </si>
-  <si>
-    <t>Appendix или нещо подобно за детайлите към тестовете (Step-by-step)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Schedule - Да се промени от 1 на няколко седмици</t>
   </si>
@@ -50,9 +35,6 @@
     <t>Да се добави Telerik Testing Studio като Tool</t>
   </si>
   <si>
-    <t>Да се добави приоритет за бъговее, кейсовете и т.н.</t>
-  </si>
-  <si>
     <t>В тест кейсовете Environment да се промени на Browser</t>
   </si>
   <si>
@@ -62,23 +44,56 @@
     <t>Може да се добави риск - Загуба на файловете в Excel при Merge</t>
   </si>
   <si>
-    <t>Note: Redirect != Open</t>
-  </si>
-  <si>
     <t>Консистентни id-та между тест кейсовете. Да се добавят абривиетури в началото на id-то според теста</t>
   </si>
   <si>
-    <t>Да се пази запис на Actual Resul-тите от всеки Build</t>
-  </si>
-  <si>
     <t>ЗАБЕЛЕЖКИ</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>Дечо</t>
+  </si>
+  <si>
+    <t>Яне</t>
+  </si>
+  <si>
+    <t>Да се пази запис на Actual Resul-тите от всеки Build (Ако минем на тестлинк е излишно)</t>
+  </si>
+  <si>
+    <t>Иван</t>
+  </si>
+  <si>
+    <t>Илвие</t>
+  </si>
+  <si>
+    <t>Димитър</t>
+  </si>
+  <si>
+    <t>Regression Testing - Да се види параграфа, имахме грешни изречения</t>
+  </si>
+  <si>
+    <t>Appendix или нещо подобно за детайлите към тестовете, казаха че не би трябвало да са толкова подробно описани в тест плана</t>
+  </si>
+  <si>
+    <t>Parse/Fail Criteria - Излишни са, дублират екзит критерия</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Да се добави Probabiliy и Owner на риска в таблицата</t>
+  </si>
+  <si>
+    <t>Да се опишат  severity и priority за бъговете</t>
+  </si>
+  <si>
+    <t>Test Plan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +113,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -149,15 +172,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -432,143 +493,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C16"/>
+  <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="B1:C3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="74.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="91.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B1" s="3"/>
       <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="3">
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+    </row>
+    <row r="12" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="D12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="D13" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>14</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
+      <c r="D14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>15</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="3">
-        <v>15</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done the easier test plan assignments. Marked them as done in the excel file "Notes.xlsx"
</commit_message>
<xml_diff>
--- a/TestPlan/Notes.xlsx
+++ b/TestPlan/Notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TestsAndPlans\TestPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TestPlan\TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -123,12 +123,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -158,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -185,9 +191,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="12" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -496,7 +509,7 @@
   <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,25 +531,25 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
+    <row r="3" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
+    <row r="4" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -573,14 +586,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+    <row r="8" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
         <v>8</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -620,14 +633,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
+    <row r="13" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
         <v>12</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="12" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved the test plan schedule
</commit_message>
<xml_diff>
--- a/TestPlan/Notes.xlsx
+++ b/TestPlan/Notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TestPlan\TestPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TestsAndPlans\TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -200,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -509,7 +509,7 @@
   <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,14 +575,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
+    <row r="7" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="12" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed Environment to Browser in TestCases.xls
</commit_message>
<xml_diff>
--- a/TestPlan/Notes.xlsx
+++ b/TestPlan/Notes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Schedule - Да се промени от 1 на няколко седмици</t>
   </si>
@@ -509,7 +509,7 @@
   <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,12 +614,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+    <row r="11" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
         <v>10</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="11" t="s">
         <v>2</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added test cases done in Telerik Test Studio for the User testing. Modified the test cases for the User testing. Modified the Note file.
</commit_message>
<xml_diff>
--- a/TestPlan/Notes.xlsx
+++ b/TestPlan/Notes.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TestsAndPlans\TestPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dimitar Panayotov\Dropbox\Git\Team Lich\TestsAndPlans\TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -509,7 +509,7 @@
   <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,14 +625,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
+    <row r="12" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -647,14 +647,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:4" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+    <row r="14" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
         <v>14</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="12" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Last minute changes made during the lecture before the presentation
</commit_message>
<xml_diff>
--- a/TestPlan/Notes.xlsx
+++ b/TestPlan/Notes.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dimitar Panayotov\Dropbox\Git\Team Lich\TestsAndPlans\TestPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decho\Desktop\TestsAndPlans\TestPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Schedule - Да се промени от 1 на няколко седмици</t>
   </si>
@@ -53,24 +53,9 @@
     <t>Test Cases</t>
   </si>
   <si>
-    <t>Дечо</t>
-  </si>
-  <si>
-    <t>Яне</t>
-  </si>
-  <si>
     <t>Да се пази запис на Actual Resul-тите от всеки Build (Ако минем на тестлинк е излишно)</t>
   </si>
   <si>
-    <t>Иван</t>
-  </si>
-  <si>
-    <t>Илвие</t>
-  </si>
-  <si>
-    <t>Димитър</t>
-  </si>
-  <si>
     <t>Regression Testing - Да се види параграфа, имахме грешни изречения</t>
   </si>
   <si>
@@ -87,13 +72,16 @@
   </si>
   <si>
     <t>Test Plan</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +110,18 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -132,7 +132,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FF70FF21"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,20 +164,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -191,16 +179,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="12" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="12" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="12" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -232,6 +226,11 @@
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF70FF21"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -506,167 +505,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="91.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="10">
+    <row r="2" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C10" s="9"/>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
+      <c r="C11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="12" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>9</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>11</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>12</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
-        <v>5</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <v>6</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="10">
-        <v>7</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
-        <v>8</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <v>9</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="10">
-        <v>10</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
-        <v>11</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="10">
-        <v>12</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="10">
-        <v>14</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
-        <v>15</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>